<commit_message>
combined groups cluster analysis Frost
-I am not really convinced of this method, especially the ASI class
-no clear trends can be seen in the combined groups
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_time_area/Frost/ASI/control_points_count.xlsx
+++ b/_CLUSTER/groups_time_area/Frost/ASI/control_points_count.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -376,22 +376,14 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1602</v>
+        <v>3061</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1459</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="n">
         <v>1197</v>
       </c>
     </row>

</xml_diff>